<commit_message>
Combining Sprint Charts & Adding Task Allocation
</commit_message>
<xml_diff>
--- a/Docs/Release Burndown Chart.xlsx
+++ b/Docs/Release Burndown Chart.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Christian\Documents\GitHub\MediaVault\Docs\Christian Guilbert\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Christian\Documents\GitHub\MediaVault\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,12 +24,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Story Points</t>
   </si>
   <si>
     <t>Sprints</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A burndown chart I created to record the teams sprint progress </t>
+  </si>
+  <si>
+    <t>throughout Release 1</t>
   </si>
 </sst>
 </file>
@@ -280,11 +286,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="470902296"/>
-        <c:axId val="470897984"/>
+        <c:axId val="541866704"/>
+        <c:axId val="541877288"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="470902296"/>
+        <c:axId val="541866704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -397,12 +403,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="470897984"/>
+        <c:crossAx val="541877288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="470897984"/>
+        <c:axId val="541877288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -515,7 +521,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="470902296"/>
+        <c:crossAx val="541866704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1418,10 +1424,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1511,6 +1517,16 @@
         <v>0</v>
       </c>
     </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>